<commit_message>
Lab 4 de algoritmia
</commit_message>
<xml_diff>
--- a/lab/lab4/p2/mediciones.xlsx
+++ b/lab/lab4/p2/mediciones.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F530AE395A1034DF323EC11741A10FA559FE5EAA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAB8DB41-DE43-472F-9A7B-AD22D40BB238}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="-21710" yWindow="7020" windowWidth="21820" windowHeight="14620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,17 +14,28 @@
     <sheet name="rapido" sheetId="3" r:id="rId4"/>
     <sheet name="Hoja4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="10">
   <si>
     <t>n</t>
   </si>
@@ -40,19 +52,25 @@
     <t>FdT</t>
   </si>
   <si>
-    <t>Caso</t>
-  </si>
-  <si>
     <t>Rapido</t>
   </si>
   <si>
     <t>Rapido + Insercion</t>
   </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>FdF</t>
+  </si>
+  <si>
+    <t>Caso (k)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -62,15 +80,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,13 +108,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -100,6 +147,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,105 +415,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C4" s="3">
         <v>10000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>611</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>1483</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>1127</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C5" s="3">
         <f>2*C4</f>
         <v>20000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>2437</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>5966</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>4507</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C6" s="3">
         <f t="shared" ref="C6:C7" si="0">2*C5</f>
         <v>40000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>9725</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>23596</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>18162</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>80000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>39589</v>
       </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8">
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="3">
         <f>2*C7</f>
         <v>160000</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -472,92 +523,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C4" s="3">
         <v>10000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>522</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>590</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>523</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C5" s="3">
         <f>2*C4</f>
         <v>20000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>2043</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>2328</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>2068</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C6" s="3">
         <f t="shared" ref="C6:C7" si="0">2*C5</f>
         <v>40000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>8241</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>9254</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>8242</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>80000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>32667</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>36604</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>32504</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="3">
         <f>2*C7</f>
         <v>160000</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -566,34 +626,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="1">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C4" s="3">
         <v>10000</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E4" s="1">
         <v>787</v>
       </c>
@@ -601,12 +663,14 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="1">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C5" s="3">
         <f>2*C4</f>
         <v>20000</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="1">
         <v>3126</v>
       </c>
@@ -614,12 +678,14 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C6" s="3">
         <f t="shared" ref="C6:C7" si="0">2*C5</f>
         <v>40000</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="1">
         <v>12544</v>
       </c>
@@ -627,12 +693,14 @@
         <v>6293</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>80000</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E7" s="1">
         <v>49917</v>
       </c>
@@ -640,85 +708,154 @@
         <v>24812</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="3">
         <f>2*C7</f>
         <v>160000</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C9" s="3">
         <f t="shared" ref="C9:C14" si="1">2*C8</f>
         <v>320000</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="3">
         <f t="shared" si="1"/>
         <v>640000</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="1">
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="3">
         <f t="shared" si="1"/>
         <v>1280000</v>
       </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1">
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="3">
         <f t="shared" si="1"/>
         <v>2560000</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="1">
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="3">
         <f>2*C12</f>
         <v>5120000</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="1">
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C14" s="3">
         <f t="shared" si="1"/>
         <v>10240000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>274</v>
       </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="1">
+      <c r="E14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="3">
         <f>2*C14</f>
         <v>20480000</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>545</v>
       </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C16" s="3">
         <f>2*C15</f>
         <v>40960000</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>1102</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+      <c r="E16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C17" s="3">
         <f>2*C16</f>
         <v>81920000</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>2216</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -728,130 +865,130 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C3:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C4" s="3">
         <v>250000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>119</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>148</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C5" s="3">
         <f>2*C4</f>
         <v>500000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>236</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>268</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>382</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C6" s="3">
         <f t="shared" ref="C6:C10" si="0">2*C5</f>
         <v>1000000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>490</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>568</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>869</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>2000000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1019</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>1176</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>2107</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>2142</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>2404</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>6000</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
         <v>8000000</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>4506</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>4988</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>17060</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="3">
         <f t="shared" si="0"/>
         <v>16000000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>9349</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>10340</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>56827</v>
       </c>
     </row>
@@ -861,107 +998,113 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>56827</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>56827</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>50275</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C6" s="3">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1">
+        <v>46126</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C7" s="3">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C8" s="3">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43020</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="3">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>30672</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="3">
+        <v>200</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8660</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>2878</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>3725</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>2892</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>3326</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <v>3137</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>100</v>
-      </c>
-      <c r="D9">
-        <v>2471</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>200</v>
-      </c>
-      <c r="D10">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11">
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C11" s="3">
         <v>500</v>
       </c>
-      <c r="D11">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12">
+      <c r="D11" s="1">
+        <v>18498</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="3">
         <v>1000</v>
       </c>
-      <c r="D12">
-        <v>1759</v>
+      <c r="D12" s="1">
+        <v>35034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>